<commit_message>
add version 2 with new data
</commit_message>
<xml_diff>
--- a/Geology Input for Petar Updated April 11th.xlsx
+++ b/Geology Input for Petar Updated April 11th.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Athos project\GeologicalCategorisation\GeoCategorisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B6B09B-7E2C-45EB-B7F6-B9E841A8B8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEB3C32-9FCC-40AD-9B48-41648E87237E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A66157AB-14BF-4491-9FF3-B6FED74962E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A66157AB-14BF-4491-9FF3-B6FED74962E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="131">
   <si>
     <t>sandstone</t>
   </si>
@@ -842,30 +842,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>weird marine plants &amp; critters</t>
-  </si>
-  <si>
-    <t>Sediment</t>
-  </si>
-  <si>
-    <t>gravel</t>
-  </si>
-  <si>
-    <t>sand</t>
-  </si>
-  <si>
-    <t>mud</t>
-  </si>
-  <si>
-    <t>Sedimentary Structures</t>
-  </si>
-  <si>
-    <t>trough bedding</t>
-  </si>
-  <si>
-    <t>cross lamination</t>
   </si>
   <si>
     <t>River Channel</t>
@@ -1310,7 +1286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1400,6 +1376,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1466,131 +1523,14 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1922,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F59F5A-2323-4ACD-B83A-9D2DE4AFC9F3}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B58"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,22 +1888,22 @@
       <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="58" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1971,18 +1911,18 @@
       <c r="B3" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="32"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="59"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="44" t="s">
         <v>120</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2005,8 +1945,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
@@ -2025,8 +1965,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="6" t="s">
         <v>65</v>
       </c>
@@ -2043,8 +1983,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="57"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -2057,7 +1997,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2067,8 +2007,8 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="58" t="s">
+      <c r="A9" s="66"/>
+      <c r="B9" s="47" t="s">
         <v>119</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2091,8 +2031,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
         <v>7</v>
@@ -2109,8 +2049,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -2123,8 +2063,8 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -2133,7 +2073,7 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2143,8 +2083,8 @@
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="61" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="50" t="s">
         <v>118</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2167,8 +2107,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="62"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="10" t="s">
         <v>17</v>
       </c>
@@ -2189,8 +2129,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="10" t="s">
         <v>74</v>
       </c>
@@ -2209,8 +2149,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -2223,7 +2163,7 @@
       <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2233,8 +2173,8 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="64" t="s">
+      <c r="A19" s="66"/>
+      <c r="B19" s="53" t="s">
         <v>117</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -2257,8 +2197,8 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="12" t="s">
         <v>18</v>
       </c>
@@ -2279,8 +2219,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -2295,8 +2235,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -2311,8 +2251,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -2323,7 +2263,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
+      <c r="A24" s="66"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2333,8 +2273,8 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="43" t="s">
+      <c r="A25" s="66"/>
+      <c r="B25" s="70" t="s">
         <v>116</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -2357,8 +2297,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="44"/>
+      <c r="A26" s="66"/>
+      <c r="B26" s="71"/>
       <c r="C26" s="13" t="s">
         <v>16</v>
       </c>
@@ -2377,8 +2317,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="44"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="71"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
@@ -2391,8 +2331,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
-      <c r="B28" s="44"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="71"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -2411,10 +2351,10 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="72" t="s">
         <v>115</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -2437,8 +2377,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
-      <c r="B31" s="46"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="15" t="s">
         <v>17</v>
       </c>
@@ -2457,8 +2397,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="46"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="15" t="s">
         <v>34</v>
       </c>
@@ -2477,8 +2417,8 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="46"/>
+      <c r="A33" s="63"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="15" t="s">
         <v>35</v>
       </c>
@@ -2497,7 +2437,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
+      <c r="A34" s="63"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2507,8 +2447,8 @@
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="47" t="s">
+      <c r="A35" s="63"/>
+      <c r="B35" s="74" t="s">
         <v>114</v>
       </c>
       <c r="C35" s="16" t="s">
@@ -2531,8 +2471,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="36"/>
-      <c r="B36" s="48"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="75"/>
       <c r="C36" s="16" t="s">
         <v>91</v>
       </c>
@@ -2551,8 +2491,8 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="48"/>
+      <c r="A37" s="63"/>
+      <c r="B37" s="75"/>
       <c r="C37" s="16"/>
       <c r="D37" s="16" t="s">
         <v>93</v>
@@ -2569,8 +2509,8 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="36"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="63"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2583,8 +2523,8 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="76"/>
       <c r="C39" s="18"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2605,10 +2545,10 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="77" t="s">
         <v>113</v>
       </c>
       <c r="C41" s="20" t="s">
@@ -2631,8 +2571,8 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="21" t="s">
         <v>17</v>
       </c>
@@ -2653,8 +2593,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="78"/>
       <c r="C43" s="21" t="s">
         <v>41</v>
       </c>
@@ -2673,8 +2613,8 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="51"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="21" t="s">
         <v>35</v>
       </c>
@@ -2691,8 +2631,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="34"/>
-      <c r="B45" s="51"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="78"/>
       <c r="C45" s="21" t="s">
         <v>16</v>
       </c>
@@ -2709,8 +2649,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="61"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
       <c r="E46" s="21"/>
@@ -2721,7 +2661,7 @@
       <c r="H46" s="21"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="34"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2732,8 +2672,8 @@
       <c r="K47" s="26"/>
     </row>
     <row r="48" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34"/>
-      <c r="B48" s="67" t="s">
+      <c r="A48" s="61"/>
+      <c r="B48" s="56" t="s">
         <v>112</v>
       </c>
       <c r="C48" s="22" t="s">
@@ -2757,8 +2697,8 @@
       <c r="K48" s="26"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
-      <c r="B49" s="68"/>
+      <c r="A49" s="61"/>
+      <c r="B49" s="57"/>
       <c r="C49" s="22" t="s">
         <v>17</v>
       </c>
@@ -2777,8 +2717,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
-      <c r="B50" s="68"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="57"/>
       <c r="C50" s="22" t="s">
         <v>41</v>
       </c>
@@ -2797,8 +2737,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
-      <c r="B51" s="68"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="57"/>
       <c r="C51" s="22" t="s">
         <v>35</v>
       </c>
@@ -2815,8 +2755,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
-      <c r="B52" s="68"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="57"/>
       <c r="C52" s="22" t="s">
         <v>16</v>
       </c>
@@ -2827,7 +2767,7 @@
       <c r="H52" s="23"/>
     </row>
     <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="34"/>
+      <c r="A53" s="61"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2837,8 +2777,8 @@
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="34"/>
-      <c r="B54" s="67" t="s">
+      <c r="A54" s="61"/>
+      <c r="B54" s="56" t="s">
         <v>111</v>
       </c>
       <c r="C54" s="24" t="s">
@@ -2861,8 +2801,8 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="34"/>
-      <c r="B55" s="68"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="57"/>
       <c r="C55" s="24" t="s">
         <v>47</v>
       </c>
@@ -2883,8 +2823,8 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="34"/>
-      <c r="B56" s="68"/>
+      <c r="A56" s="61"/>
+      <c r="B56" s="57"/>
       <c r="C56" s="24" t="s">
         <v>109</v>
       </c>
@@ -2903,8 +2843,8 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="34"/>
-      <c r="B57" s="68"/>
+      <c r="A57" s="61"/>
+      <c r="B57" s="57"/>
       <c r="C57" s="24" t="s">
         <v>110</v>
       </c>
@@ -2921,8 +2861,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
-      <c r="B58" s="68"/>
+      <c r="A58" s="61"/>
+      <c r="B58" s="57"/>
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
@@ -2937,7 +2877,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
+      <c r="A59" s="61"/>
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
@@ -2950,7 +2890,7 @@
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="53" t="s">
+      <c r="A61" s="42" t="s">
         <v>55</v>
       </c>
       <c r="B61" s="25" t="s">
@@ -2976,7 +2916,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
+      <c r="A62" s="43"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
@@ -2987,13 +2927,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B54:B58"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="A41:A59"/>
     <mergeCell ref="A30:A39"/>
@@ -3007,6 +2940,13 @@
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="B35:B39"/>
     <mergeCell ref="B41:B46"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B54:B58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3015,494 +2955,561 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB57838-DBD2-48EF-AE0F-2A28BBF6CB0A}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:A105"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="69"/>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="69"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="69"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="69"/>
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="69"/>
-      <c r="B13" s="15" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
-      <c r="B14" s="16" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="69"/>
-      <c r="B15" s="21" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
-      <c r="B16" s="24" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="24" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="69"/>
-      <c r="B19" s="6" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="69"/>
-      <c r="B20" s="10" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
-      <c r="B21" s="13" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="69"/>
-      <c r="B22" s="13" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="69"/>
-      <c r="B23" s="15" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="69"/>
-      <c r="B24" s="15" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
-      <c r="B25" s="15" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
-      <c r="B26" s="16" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
-      <c r="B27" s="21" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="69"/>
-      <c r="B28" s="24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
-      <c r="B30" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="69"/>
-      <c r="B31" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="69"/>
-      <c r="B32" s="15" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="81" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="81" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
-      <c r="B35" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
-      <c r="B36" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
-      <c r="B37" s="24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="69"/>
-      <c r="B38" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="69" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="69"/>
-      <c r="B40" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="69"/>
-      <c r="B41" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="69"/>
-      <c r="B42" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="69"/>
-      <c r="B43" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="69"/>
-      <c r="B44" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="69"/>
-      <c r="B45" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="69"/>
-      <c r="B46" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="69"/>
-      <c r="B47" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="69"/>
-      <c r="B48" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="69"/>
-      <c r="B49" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="69"/>
-      <c r="B50" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="69"/>
-      <c r="B51" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="69"/>
-      <c r="B52" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="69"/>
-      <c r="B53" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="69"/>
-      <c r="B54" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="69"/>
-      <c r="B55" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="69"/>
-      <c r="B56" s="22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="69"/>
-      <c r="B57" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="69"/>
-      <c r="B58" s="24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="69"/>
-      <c r="B59" s="24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="69"/>
-      <c r="B61" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="69"/>
-      <c r="B62" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="69"/>
-      <c r="B63" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="69"/>
-      <c r="B64" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="69"/>
-      <c r="B65" s="70" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="69"/>
-      <c r="B66" s="70" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="69"/>
-      <c r="B67" s="71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="69"/>
-      <c r="B68" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="69"/>
-      <c r="B69" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="69"/>
-      <c r="B70" s="72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="69"/>
-      <c r="B71" s="23" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="69"/>
-      <c r="B72" s="73" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="69"/>
-      <c r="B73" s="73" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="24" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:A17"/>
-    <mergeCell ref="A18:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A39:A59"/>
-    <mergeCell ref="A60:A73"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82904B34-A1B1-43E4-B464-CDF2646750E5}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I105" sqref="I1:I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
@@ -3515,13 +3522,13 @@
         <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
@@ -3534,14 +3541,14 @@
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="E2" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>0</v>
@@ -3554,14 +3561,14 @@
       <c r="B3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="E3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>4</v>
@@ -3574,14 +3581,14 @@
       <c r="B4" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>58</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E4" s="6" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>60</v>
@@ -3594,14 +3601,14 @@
       <c r="B5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>30</v>
+      <c r="D5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>3</v>
@@ -3614,13 +3621,16 @@
       <c r="B6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="70" t="s">
+      <c r="D6" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="31" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3631,11 +3641,14 @@
       <c r="B7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="70" t="s">
-        <v>32</v>
+      <c r="D7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3645,11 +3658,14 @@
       <c r="B8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>1</v>
+      <c r="D8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3659,11 +3675,14 @@
       <c r="B9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="71" t="s">
-        <v>6</v>
+      <c r="D9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3673,112 +3692,188 @@
       <c r="B10" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>40</v>
+      <c r="D10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>72</v>
+      <c r="B11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="72" t="s">
-        <v>5</v>
+      <c r="B12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>35</v>
       </c>
+      <c r="B13" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>45</v>
+        <v>89</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>37</v>
       </c>
+      <c r="B14" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="E14" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="73" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="E18" s="21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>44</v>
+      </c>
       <c r="E19" s="22" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="80" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="81" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="24" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="81" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="81" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="81" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3789,10 +3884,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299DC8EF-B1A1-4227-B6AA-92EE7CDD8EAB}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,25 +3901,33 @@
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="74" t="s">
+      <c r="C1" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="74" t="s">
+      <c r="D1" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="82" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3833,10 +3936,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2F0F45-95D1-4614-A5AC-31BC6844E1CD}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3847,203 +3950,92 @@
   <sheetData>
     <row r="1" spans="1:2" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="75" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="77" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="83" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="87" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="92" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="90" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="40" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="36" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="90" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="40" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="78"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="78"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="79"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="81"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="81"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="82"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="84"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="84"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="84"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="86"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="86"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="86"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="88"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="88"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="88"/>
-    </row>
-    <row r="36" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="89"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="93"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="93"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="93"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="93"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="94"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="91"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="91"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="91"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="91"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="91"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="91"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="91"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="91"/>
-    </row>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>